<commit_message>
Changed Student Name Spelling
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kashifdelvi/mernLearning/mernLearning/result/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nawaz\Downloads\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1379E21-470F-C648-891A-FEA5DFD4A019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D5DA3E-ABF0-4925-84B0-5A9F16FBC2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="4500" windowWidth="29740" windowHeight="20360" xr2:uid="{63D87296-F3F2-45D4-997E-522E6FCC1630}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63D87296-F3F2-45D4-997E-522E6FCC1630}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Huda National School DJ Halli</t>
   </si>
@@ -44,9 +41,6 @@
     <t>REGISTER_NO</t>
   </si>
   <si>
-    <t>STUDEN_ NAME</t>
-  </si>
-  <si>
     <t>SCHOOL_NAME</t>
   </si>
   <si>
@@ -84,6 +78,75 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Mohammed</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Ulla</t>
+  </si>
+  <si>
+    <t>Saniya</t>
+  </si>
+  <si>
+    <t>Kulsum</t>
+  </si>
+  <si>
+    <t>Amreen</t>
+  </si>
+  <si>
+    <t>Ameen</t>
+  </si>
+  <si>
+    <t>Nawaz</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Salman</t>
+  </si>
+  <si>
+    <t>Sameer</t>
+  </si>
+  <si>
+    <t>Afroz</t>
+  </si>
+  <si>
+    <t>Nadeem</t>
+  </si>
+  <si>
+    <t>Danial</t>
+  </si>
+  <si>
+    <t>Kamran</t>
+  </si>
+  <si>
+    <t>Waseem</t>
+  </si>
+  <si>
+    <t>Akif</t>
+  </si>
+  <si>
+    <t>Imran</t>
+  </si>
+  <si>
+    <t>Pasha</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Simran</t>
+  </si>
+  <si>
+    <t>STUDENT_NAME</t>
   </si>
 </sst>
 </file>
@@ -479,66 +542,68 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="16.1640625" customWidth="1"/>
+    <col min="5" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>20220102037</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,19 +635,21 @@
         <v>0.92600000000000005</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>20220102038</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2">
         <v>80</v>
@@ -592,405 +659,836 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2">
         <v>75</v>
       </c>
       <c r="J3" s="2">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="K3" s="2">
         <f>SUM(D3:J3)</f>
-        <v>424</v>
+        <v>294</v>
       </c>
       <c r="L3" s="4">
         <f>K3/500</f>
-        <v>0.84799999999999998</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>20220102039</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D4" s="2">
+        <v>75</v>
+      </c>
+      <c r="E4" s="2">
+        <v>78</v>
+      </c>
+      <c r="G4" s="3">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>75</v>
+      </c>
+      <c r="I4" s="2">
+        <v>31</v>
+      </c>
+      <c r="J4" s="2">
+        <v>75</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K23" si="0">SUM(D4:J4)</f>
+        <v>394</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L23" si="1">K4/500</f>
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>20220102040</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2">
+        <v>75</v>
+      </c>
+      <c r="G5" s="2">
+        <v>78</v>
+      </c>
+      <c r="H5" s="2">
+        <v>78</v>
+      </c>
+      <c r="I5" s="2">
+        <v>75</v>
+      </c>
+      <c r="J5" s="2">
+        <v>78</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.83</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>20220102041</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" s="2">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2">
+        <v>78</v>
+      </c>
+      <c r="G6" s="2">
+        <v>80</v>
+      </c>
+      <c r="H6" s="2">
+        <v>75</v>
+      </c>
+      <c r="I6" s="2">
+        <v>75</v>
+      </c>
+      <c r="J6" s="2">
+        <v>78</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>461</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>20220102042</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2">
+        <v>78</v>
+      </c>
+      <c r="G7" s="2">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2">
+        <v>75</v>
+      </c>
+      <c r="I7" s="2">
+        <v>31</v>
+      </c>
+      <c r="J7" s="2">
+        <v>75</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>384</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>20220102043</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2">
+        <v>75</v>
+      </c>
+      <c r="G8" s="2">
+        <v>46</v>
+      </c>
+      <c r="H8" s="2">
+        <v>90</v>
+      </c>
+      <c r="I8" s="2">
+        <v>75</v>
+      </c>
+      <c r="J8" s="2">
+        <v>78</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>442</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>20220102044</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D9" s="2">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2">
+        <v>89</v>
+      </c>
+      <c r="G9" s="2">
+        <v>78</v>
+      </c>
+      <c r="H9" s="2">
+        <v>75</v>
+      </c>
+      <c r="I9" s="2">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2">
+        <v>75</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>20220102045</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D10" s="2">
+        <v>75</v>
+      </c>
+      <c r="E10" s="2">
+        <v>78</v>
+      </c>
+      <c r="G10" s="3">
+        <v>60</v>
+      </c>
+      <c r="H10" s="2">
+        <v>75</v>
+      </c>
+      <c r="I10" s="2">
+        <v>75</v>
+      </c>
+      <c r="J10" s="2">
+        <v>78</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>20220102046</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="2">
+        <v>90</v>
+      </c>
+      <c r="E11" s="2">
+        <v>75</v>
+      </c>
+      <c r="G11" s="2">
+        <v>78</v>
+      </c>
+      <c r="H11" s="2">
+        <v>31</v>
+      </c>
+      <c r="I11" s="2">
+        <v>31</v>
+      </c>
+      <c r="J11" s="2">
+        <v>75</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>20220102047</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="D12" s="2">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <v>80</v>
+      </c>
+      <c r="H12" s="2">
+        <v>29</v>
+      </c>
+      <c r="I12" s="2">
+        <v>75</v>
+      </c>
+      <c r="J12" s="2">
+        <v>78</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>20220102048</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="2">
+        <v>75</v>
+      </c>
+      <c r="E13" s="2">
+        <v>78</v>
+      </c>
+      <c r="F13" s="2">
+        <v>50</v>
+      </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="2">
+        <v>75</v>
+      </c>
+      <c r="I13" s="2">
+        <v>75</v>
+      </c>
+      <c r="J13" s="2">
+        <v>78</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="0"/>
+        <v>431</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>20220102049</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="2">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2">
+        <v>75</v>
+      </c>
+      <c r="F14" s="2">
+        <v>46</v>
+      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H14" s="2">
+        <v>89</v>
+      </c>
+      <c r="I14" s="2">
+        <v>31</v>
+      </c>
+      <c r="J14" s="2">
+        <v>75</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="0"/>
+        <v>347</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>20220102050</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="2">
+        <v>75</v>
+      </c>
+      <c r="E15" s="2">
+        <v>89</v>
+      </c>
+      <c r="F15" s="2">
+        <v>78</v>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="2">
+        <v>78</v>
+      </c>
+      <c r="I15" s="2">
+        <v>75</v>
+      </c>
+      <c r="J15" s="2">
+        <v>78</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="0"/>
+        <v>473</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>20220102051</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="2">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2">
+        <v>75</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="2">
+        <v>75</v>
+      </c>
+      <c r="I16" s="2">
+        <v>75</v>
+      </c>
+      <c r="J16" s="2">
+        <v>78</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="0"/>
+        <v>424</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>20220102052</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="2">
+        <v>89</v>
+      </c>
+      <c r="E17" s="2">
+        <v>78</v>
+      </c>
+      <c r="F17" s="2">
+        <v>90</v>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H17" s="2">
+        <v>75</v>
+      </c>
+      <c r="I17" s="2">
+        <v>31</v>
+      </c>
+      <c r="J17" s="2">
+        <v>75</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="0"/>
+        <v>438</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.876</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>20220102053</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="2">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3">
+        <v>60</v>
+      </c>
+      <c r="F18" s="2">
+        <v>75</v>
+      </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="2">
+        <v>90</v>
+      </c>
+      <c r="I18" s="2">
+        <v>75</v>
+      </c>
+      <c r="J18" s="2">
+        <v>78</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="0"/>
+        <v>456</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>20220102054</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="2">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2">
+        <v>78</v>
+      </c>
+      <c r="F19" s="2">
+        <v>75</v>
+      </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="2">
+        <v>75</v>
+      </c>
+      <c r="I19" s="2">
+        <v>31</v>
+      </c>
+      <c r="J19" s="2">
+        <v>75</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="0"/>
+        <v>409</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>20220102055</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="2">
+        <v>78</v>
+      </c>
+      <c r="E20" s="2">
+        <v>80</v>
+      </c>
+      <c r="F20" s="2">
+        <v>31</v>
+      </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="2">
+        <v>75</v>
+      </c>
+      <c r="I20" s="2">
+        <v>75</v>
+      </c>
+      <c r="J20" s="2">
+        <v>78</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="0"/>
+        <v>417</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20220102056</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="2">
+        <v>78</v>
+      </c>
+      <c r="E21" s="2">
+        <v>50</v>
+      </c>
+      <c r="F21" s="2">
+        <v>75</v>
+      </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="2">
+        <v>65</v>
+      </c>
+      <c r="I21" s="2">
+        <v>31</v>
+      </c>
+      <c r="J21" s="2">
+        <v>75</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="0"/>
+        <v>374</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.748</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20220102057</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="D22" s="2">
+        <v>75</v>
+      </c>
+      <c r="E22" s="2">
+        <v>46</v>
+      </c>
+      <c r="F22" s="2">
+        <v>77</v>
+      </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="2">
+        <v>75</v>
+      </c>
+      <c r="I22" s="2">
+        <v>89</v>
+      </c>
+      <c r="J22" s="2">
+        <v>78</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.88</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20220102058</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="D23" s="2">
+        <v>78</v>
+      </c>
+      <c r="E23" s="2">
+        <v>89</v>
+      </c>
+      <c r="F23" s="2">
+        <v>78</v>
+      </c>
       <c r="G23" s="5"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="H23" s="2">
+        <v>75</v>
+      </c>
+      <c r="I23" s="2">
+        <v>89</v>
+      </c>
+      <c r="J23" s="2">
+        <v>78</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="0"/>
+        <v>487</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="1"/>
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update File Upload Code
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nawaz\Downloads\Archive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nawaz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D5DA3E-ABF0-4925-84B0-5A9F16FBC2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD01AC6-84C5-4EA2-9C9F-7B0C9FFC30C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63D87296-F3F2-45D4-997E-522E6FCC1630}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,31 +608,31 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H2" s="2">
         <v>70</v>
       </c>
       <c r="I2" s="2">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="K2" s="2">
         <f>SUM(D2:J2)</f>
-        <v>463</v>
+        <v>420</v>
       </c>
       <c r="L2" s="4">
         <f>K2/500</f>
-        <v>0.92600000000000005</v>
+        <v>0.84</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>13</v>

</xml_diff>